<commit_message>
Add Column names for clarity
</commit_message>
<xml_diff>
--- a/Bradford_calc_app/bradfordtest.xlsx
+++ b/Bradford_calc_app/bradfordtest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unizares-my.sharepoint.com/personal/818785_unizar_es/Documents/Laboratorio/UCL ILDH 2023/GitHub Repository UCL/UCL-ILDH-Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unizares-my.sharepoint.com/personal/818785_unizar_es/Documents/Laboratorio/UCL ILDH 2023/GitHub Repository UCL/UCL-ILDH-Results/Bradford_calc_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6E70B05-0063-4F69-8C6B-E7555C431F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{D6E70B05-0063-4F69-8C6B-E7555C431F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04539C35-E974-44B5-BE26-5A68F5DF3697}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9B347E06-041B-44F6-98F6-E8C8799DAFEB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>SNU 24h Control</t>
   </si>
@@ -84,6 +84,24 @@
   </si>
   <si>
     <t>CCLP 48h 3µM APR</t>
+  </si>
+  <si>
+    <t>BSA µg/µL</t>
+  </si>
+  <si>
+    <t>BSA Absorbances</t>
+  </si>
+  <si>
+    <t>BSA Absorbances Duplicate</t>
+  </si>
+  <si>
+    <t>Sample Names</t>
+  </si>
+  <si>
+    <t>Sample Absorbances</t>
+  </si>
+  <si>
+    <t>Sample Absorbances Duplicate</t>
   </si>
 </sst>
 </file>
@@ -505,14 +523,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5A7339-5CFA-4D90-B467-2AA82F48DA3F}">
-  <dimension ref="A2:F17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F17"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.36328125" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>

</xml_diff>